<commit_message>
Administracion de los mensajes de error mediante (Enum y tabla MENSAJES_SISTEMA)
</commit_message>
<xml_diff>
--- a/Esquema BD - Reservaciones de Habitaciones para Hoteles.xlsx
+++ b/Esquema BD - Reservaciones de Habitaciones para Hoteles.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="44">
   <si>
     <t>HABITACIONES</t>
   </si>
@@ -140,6 +140,12 @@
   </si>
   <si>
     <t>ESTADOS_RESERVACIONES</t>
+  </si>
+  <si>
+    <t>MENSAJES_SISTEMA</t>
+  </si>
+  <si>
+    <t>VACHAR(200)</t>
   </si>
 </sst>
 </file>
@@ -515,7 +521,7 @@
   <dimension ref="B3:T16"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
-      <selection activeCell="L14" sqref="L14"/>
+      <selection activeCell="R15" sqref="R15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -881,10 +887,12 @@
       <c r="M13" s="2"/>
       <c r="N13" s="2"/>
       <c r="O13" s="2"/>
-      <c r="Q13" s="3"/>
-      <c r="R13" s="3"/>
-      <c r="S13" s="3"/>
-      <c r="T13" s="3"/>
+      <c r="Q13" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="R13" s="2"/>
+      <c r="S13" s="2"/>
+      <c r="T13" s="2"/>
     </row>
     <row r="14" spans="2:20" x14ac:dyDescent="0.25">
       <c r="L14" s="1" t="s">
@@ -895,10 +903,14 @@
       </c>
       <c r="N14" s="1"/>
       <c r="O14" s="1"/>
-      <c r="Q14" s="3"/>
-      <c r="R14" s="3"/>
-      <c r="S14" s="3"/>
-      <c r="T14" s="3"/>
+      <c r="Q14" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="R14" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="S14" s="1"/>
+      <c r="T14" s="1"/>
     </row>
     <row r="15" spans="2:20" x14ac:dyDescent="0.25">
       <c r="L15" s="1" t="s">
@@ -913,10 +925,18 @@
       <c r="O15" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="Q15" s="3"/>
-      <c r="R15" s="3"/>
-      <c r="S15" s="3"/>
-      <c r="T15" s="3"/>
+      <c r="Q15" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="R15" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="S15" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="T15" s="1" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="16" spans="2:20" x14ac:dyDescent="0.25">
       <c r="L16" s="1" t="s">

</xml_diff>